<commit_message>
Add Tahoe results on T400
</commit_message>
<xml_diff>
--- a/results/TreebeardComparisonResults.xlsx
+++ b/results/TreebeardComparisonResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Copied Files\OldLaptop_E\PhDResearch\treebeard\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{546E5761-D1B7-45F4-BB8E-9777A1C0D5D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887F8831-E1F4-4C57-8D99-3160756A6AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{04E4BA04-C238-410C-B755-734F8EA30249}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{04E4BA04-C238-410C-B755-734F8EA30249}"/>
   </bookViews>
   <sheets>
     <sheet name="20240313-2 - deep" sheetId="7" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="40">
   <si>
     <t>abalone</t>
   </si>
@@ -171,6 +171,12 @@
   <si>
     <t>Speedup vs XGB (AT)</t>
   </si>
+  <si>
+    <t>Speedup (4060)3</t>
+  </si>
+  <si>
+    <t>Speedup(AT)</t>
+  </si>
 </sst>
 </file>
 
@@ -218,7 +224,34 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="33">
+  <dxfs count="37">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="15" formatCode="0.00E+00"/>
     </dxf>
@@ -266,21 +299,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="15" formatCode="0.00E+00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="15" formatCode="0.00E+00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="15" formatCode="0.00E+00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="15" formatCode="0.00E+00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="15" formatCode="0.00E+00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="15" formatCode="0.00E+00"/>
@@ -1384,7 +1402,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'holmes-20240314-2'!$T$2</c:f>
+              <c:f>'holmes-20240314-2'!$V$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1417,9 +1435,28 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
           <c:xVal>
             <c:numRef>
-              <c:f>'holmes-20240314-2'!$O$3:$O$9</c:f>
+              <c:f>'holmes-20240314-2'!$Q$3:$Q$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1449,7 +1486,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'holmes-20240314-2'!$T$3:$T$9</c:f>
+              <c:f>'holmes-20240314-2'!$V$3:$V$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1744,7 +1781,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'holmes-20240314-2'!$R$2</c:f>
+              <c:f>'holmes-20240314-2'!$T$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1777,9 +1814,37 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:xVal>
             <c:numRef>
-              <c:f>'holmes-20240314-2'!$O$3:$O$9</c:f>
+              <c:f>'holmes-20240314-2'!$Q$3:$Q$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1809,7 +1874,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'holmes-20240314-2'!$R$3:$R$9</c:f>
+              <c:f>'holmes-20240314-2'!$T$3:$T$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1849,7 +1914,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'holmes-20240314-2'!$S$2</c:f>
+              <c:f>'holmes-20240314-2'!$U$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1882,9 +1947,28 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent2"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
           <c:xVal>
             <c:numRef>
-              <c:f>'holmes-20240314-2'!$O$3:$O$9</c:f>
+              <c:f>'holmes-20240314-2'!$Q$3:$Q$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1914,7 +1998,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'holmes-20240314-2'!$S$3:$S$9</c:f>
+              <c:f>'holmes-20240314-2'!$U$3:$U$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2161,6 +2245,367 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>T400 - Treebeard (AT) vs Tahoe Speedup</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'holmes-20240314-2'!$W$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tahoe Speedup (AT)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'holmes-20240314-2'!$Q$4:$Q$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16384</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'holmes-20240314-2'!$W$4:$W$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.1433127617232186</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4966496650621854</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1637677945761413</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.4676930945165232</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5832987117955089</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5074528972376151</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3149-48AB-AB20-FA97D61812C5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="747932144"/>
+        <c:axId val="747932624"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="747932144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="747932624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="747932624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="747932144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2743,6 +3188,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4808,6 +5293,522 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5404,13 +6405,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>375285</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>137160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>386715</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>137160</xdr:rowOff>
@@ -5440,13 +6441,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>61912</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>138112</xdr:rowOff>
@@ -5469,6 +6470,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3075DDF-396C-1850-7524-F45D038B8C56}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5525,57 +6562,64 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B2DC67BB-06E4-4502-B5BC-709DF4E7BA0C}" name="Table5" displayName="Table5" ref="A1:P57" totalsRowShown="0" headerRowDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B2DC67BB-06E4-4502-B5BC-709DF4E7BA0C}" name="Table5" displayName="Table5" ref="A1:P57" totalsRowShown="0" headerRowDxfId="36">
   <autoFilter ref="A1:P57" xr:uid="{B2DC67BB-06E4-4502-B5BC-709DF4E7BA0C}"/>
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{E2375FC3-1089-4119-8184-3734B94F546B}" name="Benchmark"/>
     <tableColumn id="2" xr3:uid="{75838CF2-A86D-4A18-96B2-661BE69343B2}" name="Batch size"/>
-    <tableColumn id="3" xr3:uid="{6C5A6301-02FB-4FE2-AAEB-2015F3807C11}" name="RAPIDS (Total)" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{68F1A067-8DD9-4516-9299-4A85859FA013}" name="TB (4060)" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{1C7F1EAC-83E3-4978-9C19-4A3F0F05D1C5}" name="TB (AT)" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{6C5A6301-02FB-4FE2-AAEB-2015F3807C11}" name="RAPIDS (Total)" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{68F1A067-8DD9-4516-9299-4A85859FA013}" name="TB (4060)" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{1C7F1EAC-83E3-4978-9C19-4A3F0F05D1C5}" name="TB (AT)" dataDxfId="33"/>
     <tableColumn id="6" xr3:uid="{3EBEE837-62CE-4E37-8D5E-7D4E787B098A}" name="Speedup (4060)"/>
     <tableColumn id="7" xr3:uid="{EC6BF235-4783-4F12-8893-207E5E311171}" name="Speedup (AT)"/>
-    <tableColumn id="8" xr3:uid="{4720ED76-00AB-4152-B308-94B20FAE299F}" name="RAPIDS (kernel)" dataDxfId="28"/>
-    <tableColumn id="9" xr3:uid="{D4514ED5-0334-498D-999D-AD0834D7F673}" name="TB Kernel(4060)" dataDxfId="27"/>
-    <tableColumn id="10" xr3:uid="{CB03677E-F369-4ED7-AA49-3E50F95C684C}" name="TB Kernel (AT)" dataDxfId="26"/>
+    <tableColumn id="8" xr3:uid="{4720ED76-00AB-4152-B308-94B20FAE299F}" name="RAPIDS (kernel)" dataDxfId="32"/>
+    <tableColumn id="9" xr3:uid="{D4514ED5-0334-498D-999D-AD0834D7F673}" name="TB Kernel(4060)" dataDxfId="31"/>
+    <tableColumn id="10" xr3:uid="{CB03677E-F369-4ED7-AA49-3E50F95C684C}" name="TB Kernel (AT)" dataDxfId="30"/>
     <tableColumn id="11" xr3:uid="{85303999-08FC-4FC6-A135-69C1DFA93300}" name="Speedup (4060)2"/>
     <tableColumn id="12" xr3:uid="{D14B419F-D760-426A-A16A-04D24839BF35}" name="Speedup (AT)2"/>
-    <tableColumn id="13" xr3:uid="{09712D9D-4BD0-48F2-86D4-2121EA2ADAB2}" name="Tahoe" dataDxfId="25"/>
-    <tableColumn id="14" xr3:uid="{4B2C9AD2-D289-4BC2-B164-241F3A7692CA}" name="Tahoe Speedup" dataDxfId="24">
+    <tableColumn id="13" xr3:uid="{09712D9D-4BD0-48F2-86D4-2121EA2ADAB2}" name="Tahoe" dataDxfId="29"/>
+    <tableColumn id="14" xr3:uid="{4B2C9AD2-D289-4BC2-B164-241F3A7692CA}" name="Tahoe Speedup" dataDxfId="28">
       <calculatedColumnFormula>M2/I2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{3DCAFEBE-140A-4DBE-8E0E-C7E4F0C8AA80}" name="Tahoe Speedup (AT)" dataDxfId="23">
+    <tableColumn id="15" xr3:uid="{3DCAFEBE-140A-4DBE-8E0E-C7E4F0C8AA80}" name="Tahoe Speedup (AT)" dataDxfId="27">
       <calculatedColumnFormula>M2/J2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{484BFD10-0C06-4309-858A-3018C099A1D0}" name="Tahoe-2" dataDxfId="22"/>
+    <tableColumn id="16" xr3:uid="{484BFD10-0C06-4309-858A-3018C099A1D0}" name="Tahoe-2" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{874B55A2-157C-4049-BF6C-BE43E5D16616}" name="Table6" displayName="Table6" ref="A1:L58" totalsRowCount="1" headerRowDxfId="14">
-  <autoFilter ref="A1:L57" xr:uid="{874B55A2-157C-4049-BF6C-BE43E5D16616}"/>
-  <tableColumns count="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{874B55A2-157C-4049-BF6C-BE43E5D16616}" name="Table6" displayName="Table6" ref="A1:O58" totalsRowCount="1" headerRowDxfId="25">
+  <autoFilter ref="A1:O57" xr:uid="{874B55A2-157C-4049-BF6C-BE43E5D16616}"/>
+  <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{E2D590CB-B8EC-4A13-AAF2-5488EA5BF7F1}" name="Benchmark"/>
     <tableColumn id="2" xr3:uid="{6304E35B-EF5B-4F15-AE1E-313B2235BC54}" name="Batch size"/>
-    <tableColumn id="3" xr3:uid="{321E3803-58DF-4042-94C5-066AF42AA77C}" name="RAPIDS (Total)" dataDxfId="21" totalsRowDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{96494333-E5FA-4355-90A6-59C5F9E1F5D4}" name="TB (4060)" dataDxfId="20" totalsRowDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{F2D794E9-FCC1-4E3D-93E6-F3CDAF43106D}" name="TB (AT)" dataDxfId="19" totalsRowDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{321E3803-58DF-4042-94C5-066AF42AA77C}" name="RAPIDS (Total)" dataDxfId="15" totalsRowDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{96494333-E5FA-4355-90A6-59C5F9E1F5D4}" name="TB (4060)" dataDxfId="14" totalsRowDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{F2D794E9-FCC1-4E3D-93E6-F3CDAF43106D}" name="TB (AT)" dataDxfId="13" totalsRowDxfId="4"/>
     <tableColumn id="6" xr3:uid="{E56BDC2A-1548-453C-B973-912294AA8759}" name="Speedup (4060)" totalsRowFunction="custom">
       <totalsRowFormula>GEOMEAN(F50:F57)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{C9F5C755-68BD-4B6A-A488-55B0C9A7521B}" name="Speedup (AT)" totalsRowFunction="custom">
       <totalsRowFormula>GEOMEAN(G50:G57)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{AF39F754-9B25-44A4-A2CA-41B7611C11FE}" name="RAPIDS (kernel)" dataDxfId="18" totalsRowDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{3F4C4175-3133-4FE7-9F20-D1DF972385E0}" name="TB Kernel(4060)" dataDxfId="17" totalsRowDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{55231866-9A4A-4089-9017-7BE297219880}" name="TB Kernel (AT)" dataDxfId="16" totalsRowDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{AF39F754-9B25-44A4-A2CA-41B7611C11FE}" name="RAPIDS (kernel)" dataDxfId="12" totalsRowDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{3F4C4175-3133-4FE7-9F20-D1DF972385E0}" name="TB Kernel(4060)" dataDxfId="11" totalsRowDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{55231866-9A4A-4089-9017-7BE297219880}" name="TB Kernel (AT)" dataDxfId="10" totalsRowDxfId="1"/>
     <tableColumn id="11" xr3:uid="{205F7818-0F37-4ED8-8828-FE9EB5C08490}" name="Speedup (4060)2" totalsRowFunction="custom">
       <totalsRowFormula>GEOMEAN(K50:K57)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="12" xr3:uid="{E8859735-00B1-44B3-B48B-431D7F66BC4F}" name="Speedup (AT)2" totalsRowFunction="custom">
       <totalsRowFormula>GEOMEAN(L50:L57)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="13" xr3:uid="{CD077731-21C9-44D7-950B-DC5BF85B6B75}" name="Tahoe" dataDxfId="9"/>
+    <tableColumn id="14" xr3:uid="{144131F0-3499-4AE4-9778-DEB3928BAD9D}" name="Speedup (4060)3" dataDxfId="8">
+      <calculatedColumnFormula>M2/I2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="15" xr3:uid="{A4362647-5D8B-4796-860C-729CA410492E}" name="Speedup(AT)" dataDxfId="7">
+      <calculatedColumnFormula>M2/J2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5583,16 +6627,19 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{0D1B15D7-F606-4A05-B6D4-F74339745056}" name="Table7" displayName="Table7" ref="O2:T9" totalsRowShown="0">
-  <autoFilter ref="O2:T9" xr:uid="{0D1B15D7-F606-4A05-B6D4-F74339745056}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{0D1B15D7-F606-4A05-B6D4-F74339745056}" name="Table7" displayName="Table7" ref="Q2:W9" totalsRowShown="0">
+  <autoFilter ref="Q2:W9" xr:uid="{0D1B15D7-F606-4A05-B6D4-F74339745056}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{82F43E05-EC66-4DD9-9361-6A87E826A74A}" name="Batch Size"/>
     <tableColumn id="2" xr3:uid="{85AAB8A3-F9D1-4F70-9D18-9E39AAC64C24}" name="Total Speedup"/>
     <tableColumn id="3" xr3:uid="{B39D87CE-EFC6-4FA6-9E3A-52B9668CE1D3}" name="Kernel Speedup"/>
     <tableColumn id="4" xr3:uid="{68131D1D-A4DE-40DC-9F74-BE50159B3E4C}" name="AT Total Speedup"/>
     <tableColumn id="5" xr3:uid="{177C0B75-8D84-4646-864A-60F1C1E42851}" name="AT Kernel Speedup"/>
-    <tableColumn id="6" xr3:uid="{5A4BAD27-80A7-46F2-9D76-FAFC3C512964}" name="AT Speedup" dataDxfId="15">
-      <calculatedColumnFormula>S3/Q3</calculatedColumnFormula>
+    <tableColumn id="6" xr3:uid="{5A4BAD27-80A7-46F2-9D76-FAFC3C512964}" name="AT Speedup" dataDxfId="24">
+      <calculatedColumnFormula>U3/S3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{0506A446-23B0-444E-A0AE-5FBA3154B7CB}" name="Tahoe Speedup (AT)" dataDxfId="0">
+      <calculatedColumnFormula>GEOMEAN(O9:O16)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5600,22 +6647,22 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{FDF80652-8CEA-464D-A371-E0AD54FC2D29}" name="Table10" displayName="Table10" ref="A1:O57" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{FDF80652-8CEA-464D-A371-E0AD54FC2D29}" name="Table10" displayName="Table10" ref="A1:O57" totalsRowShown="0" headerRowDxfId="23">
   <autoFilter ref="A1:O57" xr:uid="{FDF80652-8CEA-464D-A371-E0AD54FC2D29}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{5E1B41EB-0E5D-4B35-A35A-E5B662D56CE6}" name="Benchmark"/>
     <tableColumn id="2" xr3:uid="{D79CB92D-FB39-4668-8876-3EB4EC741BF6}" name="Batch size"/>
-    <tableColumn id="3" xr3:uid="{B75C0F4F-C491-4756-9B6E-1DB140F2900E}" name="XGB total" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{4FAB59A6-D2A3-4DB9-AD8D-78ED11DA17B3}" name="RAPIDS (Total)" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{F7A6F91F-D155-4A95-AE49-CE95AF33A96E}" name="TB (4060)" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{0A9FEB80-3810-42C7-AF6B-C1D231CD92F9}" name="TB (AT)" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{B75C0F4F-C491-4756-9B6E-1DB140F2900E}" name="XGB total" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{4FAB59A6-D2A3-4DB9-AD8D-78ED11DA17B3}" name="RAPIDS (Total)" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{F7A6F91F-D155-4A95-AE49-CE95AF33A96E}" name="TB (4060)" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{0A9FEB80-3810-42C7-AF6B-C1D231CD92F9}" name="TB (AT)" dataDxfId="19"/>
     <tableColumn id="7" xr3:uid="{A67EC704-ED8A-4FEA-B68B-1ADE4DDDBDE0}" name="Speedup vs XGB (4060)"/>
     <tableColumn id="8" xr3:uid="{7F009CCD-9B17-49C6-85C3-A50B5020679A}" name="Speedup vs XGB (AT)"/>
     <tableColumn id="9" xr3:uid="{34C5B7E1-C8E0-4539-A7C5-49B8646A0F4E}" name="Speedup (4060)"/>
     <tableColumn id="10" xr3:uid="{CBE1437A-9AB4-41BE-AD8E-9DA09B7301AE}" name="Speedup (AT)"/>
-    <tableColumn id="11" xr3:uid="{D80EF35B-C38D-47B0-A64D-0008726BD6D4}" name="RAPIDS (kernel)" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{92304DC3-B14A-4A19-9491-A5BF46EF5C80}" name="TB Kernel(4060)" dataDxfId="1"/>
-    <tableColumn id="13" xr3:uid="{507D8400-BD7B-416A-8BA8-3D43DD81CDB1}" name="TB Kernel (AT)" dataDxfId="0"/>
+    <tableColumn id="11" xr3:uid="{D80EF35B-C38D-47B0-A64D-0008726BD6D4}" name="RAPIDS (kernel)" dataDxfId="18"/>
+    <tableColumn id="12" xr3:uid="{92304DC3-B14A-4A19-9491-A5BF46EF5C80}" name="TB Kernel(4060)" dataDxfId="17"/>
+    <tableColumn id="13" xr3:uid="{507D8400-BD7B-416A-8BA8-3D43DD81CDB1}" name="TB Kernel (AT)" dataDxfId="16"/>
     <tableColumn id="14" xr3:uid="{2DB16934-2400-46EB-81FA-972C63EDC37C}" name="Speedup (4060)2"/>
     <tableColumn id="15" xr3:uid="{3F759732-037C-4F50-8D7B-263C80C9E3DB}" name="Speedup (AT)2"/>
   </tableColumns>
@@ -9049,10 +10096,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E012CCA-A5BF-4CA6-9836-3078D3226C07}">
-  <dimension ref="A1:T58"/>
+  <dimension ref="A1:W58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:L1"/>
+    <sheetView tabSelected="1" topLeftCell="D28" workbookViewId="0">
+      <selection activeCell="Q49" sqref="Q49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9061,14 +10108,16 @@
     <col min="2" max="9" width="9.85546875" customWidth="1"/>
     <col min="10" max="12" width="10.85546875" customWidth="1"/>
     <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.85546875" customWidth="1"/>
-    <col min="16" max="16" width="14.140625" customWidth="1"/>
-    <col min="17" max="17" width="15.42578125" customWidth="1"/>
-    <col min="18" max="18" width="16.42578125" customWidth="1"/>
-    <col min="19" max="19" width="17.7109375" customWidth="1"/>
+    <col min="14" max="14" width="9.28515625" customWidth="1"/>
+    <col min="17" max="17" width="10.85546875" customWidth="1"/>
+    <col min="18" max="18" width="14.140625" customWidth="1"/>
+    <col min="19" max="19" width="15.42578125" customWidth="1"/>
+    <col min="20" max="20" width="16.42578125" customWidth="1"/>
+    <col min="21" max="21" width="17.7109375" customWidth="1"/>
+    <col min="23" max="23" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -9105,8 +10154,18 @@
       <c r="L1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="M1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -9143,26 +10202,39 @@
       <c r="L2">
         <v>2.8041125044808601</v>
       </c>
-      <c r="O2" t="s">
+      <c r="M2" s="1"/>
+      <c r="N2" s="1">
+        <f t="shared" ref="N2:N33" si="0">M2/I2</f>
+        <v>0</v>
+      </c>
+      <c r="O2" s="1">
+        <f t="shared" ref="O2:O33" si="1">M2/J2</f>
+        <v>0</v>
+      </c>
+      <c r="P2" s="1"/>
+      <c r="Q2" t="s">
         <v>12</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>14</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>15</v>
       </c>
-      <c r="S2" t="s">
+      <c r="U2" t="s">
         <v>16</v>
       </c>
-      <c r="T2" t="s">
+      <c r="V2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -9199,27 +10271,41 @@
       <c r="L3">
         <v>12.810368521607201</v>
       </c>
-      <c r="O3">
+      <c r="M3" s="1"/>
+      <c r="N3" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O3" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P3" s="1"/>
+      <c r="Q3">
         <v>256</v>
       </c>
-      <c r="P3">
+      <c r="R3">
         <v>2.5511740034734798</v>
       </c>
-      <c r="Q3">
+      <c r="S3">
         <v>3.6149675884408401</v>
       </c>
-      <c r="R3">
+      <c r="T3">
         <v>2.7220683744394298</v>
       </c>
-      <c r="S3">
+      <c r="U3">
         <v>4.2902233361009001</v>
       </c>
-      <c r="T3">
-        <f t="shared" ref="T3:T9" si="0">S3/Q3</f>
+      <c r="V3">
+        <f t="shared" ref="V3:V9" si="2">U3/S3</f>
         <v>1.1867944127132002</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W3" t="e">
+        <f t="shared" ref="W3:W9" si="3">GEOMEAN(O9:O16)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -9256,27 +10342,41 @@
       <c r="L4">
         <v>2.5258168684026998</v>
       </c>
-      <c r="O4">
+      <c r="M4" s="1"/>
+      <c r="N4" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P4" s="1"/>
+      <c r="Q4">
         <v>512</v>
       </c>
-      <c r="P4">
+      <c r="R4">
         <v>2.4519557209494098</v>
       </c>
-      <c r="Q4">
+      <c r="S4">
         <v>3.19642756802341</v>
       </c>
-      <c r="R4">
+      <c r="T4">
         <v>2.57367514596775</v>
       </c>
-      <c r="S4">
+      <c r="U4">
         <v>3.78310568314589</v>
       </c>
-      <c r="T4">
-        <f t="shared" si="0"/>
+      <c r="V4">
+        <f t="shared" si="2"/>
         <v>1.1835418143027927</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W4">
+        <f t="shared" si="3"/>
+        <v>2.1433127617232186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -9313,27 +10413,41 @@
       <c r="L5">
         <v>2.9942040380570201</v>
       </c>
-      <c r="O5">
+      <c r="M5" s="1"/>
+      <c r="N5" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P5" s="1"/>
+      <c r="Q5">
         <v>1024</v>
       </c>
-      <c r="P5">
+      <c r="R5">
         <v>2.2797134963241601</v>
       </c>
-      <c r="Q5">
+      <c r="S5">
         <v>2.86330008043053</v>
       </c>
-      <c r="R5">
+      <c r="T5">
         <v>2.3792471829872501</v>
       </c>
-      <c r="S5">
+      <c r="U5">
         <v>3.30925544907215</v>
       </c>
-      <c r="T5">
-        <f t="shared" si="0"/>
+      <c r="V5">
+        <f t="shared" si="2"/>
         <v>1.1557487361138081</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W5">
+        <f>GEOMEAN(O18:O25)</f>
+        <v>1.4966496650621854</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -9370,27 +10484,41 @@
       <c r="L6">
         <v>3.2444643501259001</v>
       </c>
-      <c r="O6">
+      <c r="M6" s="1"/>
+      <c r="N6" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O6" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P6" s="1"/>
+      <c r="Q6">
         <v>2048</v>
       </c>
-      <c r="P6">
+      <c r="R6">
         <v>2.1583620868626499</v>
       </c>
-      <c r="Q6">
+      <c r="S6">
         <v>2.6689176150671901</v>
       </c>
-      <c r="R6">
+      <c r="T6">
         <v>2.2365109877850502</v>
       </c>
-      <c r="S6">
+      <c r="U6">
         <v>3.0101378825987601</v>
       </c>
-      <c r="T6">
-        <f t="shared" si="0"/>
+      <c r="V6">
+        <f t="shared" si="2"/>
         <v>1.127849681685652</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W6">
+        <f>GEOMEAN(O26:O33)</f>
+        <v>2.1637677945761413</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -9427,27 +10555,41 @@
       <c r="L7">
         <v>11.4329383068781</v>
       </c>
-      <c r="O7">
+      <c r="M7" s="1"/>
+      <c r="N7" s="1">
+        <f>M7/I7</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="1">
+        <f>M7/J7</f>
+        <v>0</v>
+      </c>
+      <c r="P7" s="1"/>
+      <c r="Q7">
         <v>4096</v>
       </c>
-      <c r="P7">
+      <c r="R7">
         <v>1.8551953319026</v>
       </c>
-      <c r="Q7">
+      <c r="S7">
         <v>2.3113489873513702</v>
       </c>
-      <c r="R7">
+      <c r="T7">
         <v>1.9579388666323301</v>
       </c>
-      <c r="S7">
+      <c r="U7">
         <v>2.5326857205575002</v>
       </c>
-      <c r="T7">
-        <f t="shared" si="0"/>
+      <c r="V7">
+        <f t="shared" si="2"/>
         <v>1.0957608454704908</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W7">
+        <f>GEOMEAN(O34:O41)</f>
+        <v>2.4676930945165232</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -9484,27 +10626,41 @@
       <c r="L8">
         <v>0.91751156177584903</v>
       </c>
-      <c r="O8">
+      <c r="M8" s="1"/>
+      <c r="N8" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P8" s="1"/>
+      <c r="Q8">
         <v>8192</v>
       </c>
-      <c r="P8">
+      <c r="R8">
         <v>1.95161342485072</v>
       </c>
-      <c r="Q8">
+      <c r="S8">
         <v>2.29665367753211</v>
       </c>
-      <c r="R8">
+      <c r="T8">
         <v>2.1819871159753101</v>
       </c>
-      <c r="S8">
+      <c r="U8">
         <v>2.5667604731948299</v>
       </c>
-      <c r="T8">
-        <f t="shared" si="0"/>
+      <c r="V8">
+        <f t="shared" si="2"/>
         <v>1.1176088490420399</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W8">
+        <f>GEOMEAN(O42:O49)</f>
+        <v>2.5832987117955089</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -9541,27 +10697,41 @@
       <c r="L9">
         <v>12.413278121935001</v>
       </c>
-      <c r="O9">
+      <c r="M9" s="1"/>
+      <c r="N9" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O9" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P9" s="1"/>
+      <c r="Q9">
         <v>16384</v>
       </c>
-      <c r="P9">
+      <c r="R9">
         <v>2.0470791911831259</v>
       </c>
-      <c r="Q9">
+      <c r="S9">
         <v>2.4892127403180586</v>
       </c>
-      <c r="R9">
+      <c r="T9">
         <v>2.1191621524225304</v>
       </c>
-      <c r="S9">
+      <c r="U9">
         <v>2.6316440592916504</v>
       </c>
-      <c r="T9">
-        <f t="shared" si="0"/>
+      <c r="V9">
+        <f t="shared" si="2"/>
         <v>1.0572194239032349</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W9">
+        <f>GEOMEAN(O50:O57)</f>
+        <v>2.5074528972376151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -9598,8 +10768,20 @@
       <c r="L10">
         <v>2.1641083826702099</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="M10" s="1">
+        <v>5.1199200000000002E-7</v>
+      </c>
+      <c r="N10" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2627806764394309</v>
+      </c>
+      <c r="O10" s="1">
+        <f t="shared" si="1"/>
+        <v>1.1317353757018302</v>
+      </c>
+      <c r="P10" s="1"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -9636,8 +10818,20 @@
       <c r="L11">
         <v>9.8676202532442794</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="M11" s="1">
+        <v>1.4581999999999999E-7</v>
+      </c>
+      <c r="N11" s="1">
+        <f t="shared" si="0"/>
+        <v>2.4175256413369923</v>
+      </c>
+      <c r="O11" s="1">
+        <f t="shared" si="1"/>
+        <v>2.3933718908031096</v>
+      </c>
+      <c r="P11" s="1"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -9674,8 +10868,20 @@
       <c r="L12">
         <v>2.0458663940966799</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="M12" s="1">
+        <v>1.325338E-6</v>
+      </c>
+      <c r="N12" s="1">
+        <f t="shared" si="0"/>
+        <v>2.0625895534070122</v>
+      </c>
+      <c r="O12" s="1">
+        <f t="shared" si="1"/>
+        <v>2.2572158047970805</v>
+      </c>
+      <c r="P12" s="1"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -9712,8 +10918,20 @@
       <c r="L13">
         <v>2.8370780932385502</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="M13" s="1">
+        <v>1.267103E-6</v>
+      </c>
+      <c r="N13" s="1">
+        <f t="shared" si="0"/>
+        <v>2.0312723543963358</v>
+      </c>
+      <c r="O13" s="1">
+        <f t="shared" si="1"/>
+        <v>2.630579222187869</v>
+      </c>
+      <c r="P13" s="1"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -9750,8 +10968,20 @@
       <c r="L14">
         <v>2.2885638124665499</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="M14" s="1">
+        <v>3.3417999999999999E-7</v>
+      </c>
+      <c r="N14" s="1">
+        <f t="shared" si="0"/>
+        <v>0.52436818825750409</v>
+      </c>
+      <c r="O14" s="1">
+        <f t="shared" si="1"/>
+        <v>1.0552108929402924</v>
+      </c>
+      <c r="P14" s="1"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -9788,8 +11018,20 @@
       <c r="L15">
         <v>8.6728574971965102</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="M15" s="1">
+        <v>1.5053399999999999E-7</v>
+      </c>
+      <c r="N15" s="1">
+        <f>M15/I15</f>
+        <v>2.158606588215525</v>
+      </c>
+      <c r="O15" s="1">
+        <f>M15/J15</f>
+        <v>2.1493512678157698</v>
+      </c>
+      <c r="P15" s="1"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -9826,8 +11068,20 @@
       <c r="L16">
         <v>0.72589907013812305</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16" s="1">
+        <v>6.9233870999999995E-5</v>
+      </c>
+      <c r="N16" s="1">
+        <f t="shared" si="0"/>
+        <v>2.3573959136976335</v>
+      </c>
+      <c r="O16" s="1">
+        <f t="shared" si="1"/>
+        <v>2.22110604668066</v>
+      </c>
+      <c r="P16" s="1"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -9864,8 +11118,20 @@
       <c r="L17">
         <v>8.5880566751004501</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17" s="1">
+        <v>3.99362E-7</v>
+      </c>
+      <c r="N17" s="1">
+        <f t="shared" si="0"/>
+        <v>3.4644021263527969</v>
+      </c>
+      <c r="O17" s="1">
+        <f t="shared" si="1"/>
+        <v>5.4965337036995585</v>
+      </c>
+      <c r="P17" s="1"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -9902,8 +11168,20 @@
       <c r="L18">
         <v>1.9026536513635</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18" s="1">
+        <v>4.8023799999999996E-7</v>
+      </c>
+      <c r="N18" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4391552330579449</v>
+      </c>
+      <c r="O18" s="1">
+        <f t="shared" si="1"/>
+        <v>1.1317452247790145</v>
+      </c>
+      <c r="P18" s="1"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -9940,8 +11218,20 @@
       <c r="L19">
         <v>6.0347821999899303</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19" s="1">
+        <v>1.42487E-7</v>
+      </c>
+      <c r="N19" s="1">
+        <f t="shared" si="0"/>
+        <v>2.6267434773243847</v>
+      </c>
+      <c r="O19" s="1">
+        <f t="shared" si="1"/>
+        <v>2.6282389984688823</v>
+      </c>
+      <c r="P19" s="1"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -9978,8 +11268,20 @@
       <c r="L20">
         <v>1.8416885228720701</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M20" s="1">
+        <v>1.3011910000000001E-6</v>
+      </c>
+      <c r="N20" s="1">
+        <f t="shared" si="0"/>
+        <v>2.3278293382850292</v>
+      </c>
+      <c r="O20" s="1">
+        <f t="shared" si="1"/>
+        <v>2.3376975924522485</v>
+      </c>
+      <c r="P20" s="1"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -10016,8 +11318,20 @@
       <c r="L21">
         <v>2.54386010572034</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M21" s="1">
+        <v>1.238727E-6</v>
+      </c>
+      <c r="N21" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5125401903494859</v>
+      </c>
+      <c r="O21" s="1">
+        <f t="shared" si="1"/>
+        <v>2.6940184293025342</v>
+      </c>
+      <c r="P21" s="1"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -10054,8 +11368,20 @@
       <c r="L22">
         <v>1.64489633904642</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M22" s="1">
+        <v>3.3244499999999997E-8</v>
+      </c>
+      <c r="N22" s="1">
+        <f t="shared" si="0"/>
+        <v>6.5394499702935122E-2</v>
+      </c>
+      <c r="O22" s="1">
+        <f t="shared" si="1"/>
+        <v>0.1005485103427107</v>
+      </c>
+      <c r="P22" s="1"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -10092,8 +11418,20 @@
       <c r="L23">
         <v>5.2452892026288804</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M23" s="1">
+        <v>1.4529E-7</v>
+      </c>
+      <c r="N23" s="1">
+        <f t="shared" si="0"/>
+        <v>2.2942210864872039</v>
+      </c>
+      <c r="O23" s="1">
+        <f t="shared" si="1"/>
+        <v>2.2859748780394114</v>
+      </c>
+      <c r="P23" s="1"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -10130,8 +11468,20 @@
       <c r="L24">
         <v>0.75240852538198399</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M24" s="1">
+        <v>3.4335616999999997E-5</v>
+      </c>
+      <c r="N24" s="1">
+        <f t="shared" si="0"/>
+        <v>1.169506643189516</v>
+      </c>
+      <c r="O24" s="1">
+        <f t="shared" si="1"/>
+        <v>1.1746369716762972</v>
+      </c>
+      <c r="P24" s="1"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -10168,8 +11518,20 @@
       <c r="L25">
         <v>4.8401521977291502</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M25" s="1">
+        <v>3.4672200000000003E-7</v>
+      </c>
+      <c r="N25" s="1">
+        <f t="shared" si="0"/>
+        <v>4.9523818268770938</v>
+      </c>
+      <c r="O25" s="1">
+        <f t="shared" si="1"/>
+        <v>4.9774630473477233</v>
+      </c>
+      <c r="P25" s="1"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -10206,8 +11568,20 @@
       <c r="L26">
         <v>1.77361104591255</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M26" s="1">
+        <v>4.7989900000000003E-7</v>
+      </c>
+      <c r="N26" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4114583565255434</v>
+      </c>
+      <c r="O26" s="1">
+        <f t="shared" si="1"/>
+        <v>1.1823752296654546</v>
+      </c>
+      <c r="P26" s="1"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -10244,8 +11618,20 @@
       <c r="L27">
         <v>4.9418078965979699</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M27" s="1">
+        <v>1.3839200000000001E-7</v>
+      </c>
+      <c r="N27" s="1">
+        <f t="shared" si="0"/>
+        <v>2.8843476460037403</v>
+      </c>
+      <c r="O27" s="1">
+        <f t="shared" si="1"/>
+        <v>2.8583137242048737</v>
+      </c>
+      <c r="P27" s="1"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -10282,8 +11668,20 @@
       <c r="L28">
         <v>1.6869368412757699</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M28" s="1">
+        <v>1.3070430000000001E-6</v>
+      </c>
+      <c r="N28" s="1">
+        <f t="shared" si="0"/>
+        <v>2.194850451670523</v>
+      </c>
+      <c r="O28" s="1">
+        <f t="shared" si="1"/>
+        <v>2.3399604348486478</v>
+      </c>
+      <c r="P28" s="1"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -10320,8 +11718,20 @@
       <c r="L29">
         <v>2.5408874593893098</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M29" s="1">
+        <v>1.230226E-6</v>
+      </c>
+      <c r="N29" s="1">
+        <f t="shared" si="0"/>
+        <v>2.0213300539963437</v>
+      </c>
+      <c r="O29" s="1">
+        <f t="shared" si="1"/>
+        <v>2.8696109245169041</v>
+      </c>
+      <c r="P29" s="1"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -10358,8 +11768,20 @@
       <c r="L30">
         <v>1.3777930311025099</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M30" s="1">
+        <v>3.3144499999999999E-7</v>
+      </c>
+      <c r="N30" s="1">
+        <f t="shared" si="0"/>
+        <v>0.92042359231759419</v>
+      </c>
+      <c r="O30" s="1">
+        <f t="shared" si="1"/>
+        <v>1.0042908668576067</v>
+      </c>
+      <c r="P30" s="1"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -10396,8 +11818,20 @@
       <c r="L31">
         <v>4.3189335801137698</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M31" s="1">
+        <v>1.4901399999999999E-7</v>
+      </c>
+      <c r="N31" s="1">
+        <f t="shared" si="0"/>
+        <v>2.6359997293581627</v>
+      </c>
+      <c r="O31" s="1">
+        <f t="shared" si="1"/>
+        <v>2.6318415678214309</v>
+      </c>
+      <c r="P31" s="1"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -10434,8 +11868,20 @@
       <c r="L32">
         <v>0.78484075652009799</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M32" s="1">
+        <v>3.6062534000000002E-5</v>
+      </c>
+      <c r="N32" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2586806758687579</v>
+      </c>
+      <c r="O32" s="1">
+        <f t="shared" si="1"/>
+        <v>1.2647270882507207</v>
+      </c>
+      <c r="P32" s="1"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -10472,8 +11918,20 @@
       <c r="L33">
         <v>3.95427512862081</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M33" s="1">
+        <v>3.9159799999999998E-7</v>
+      </c>
+      <c r="N33" s="1">
+        <f t="shared" si="0"/>
+        <v>5.9808358256816598</v>
+      </c>
+      <c r="O33" s="1">
+        <f t="shared" si="1"/>
+        <v>6.333917401648649</v>
+      </c>
+      <c r="P33" s="1"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>0</v>
       </c>
@@ -10510,8 +11968,20 @@
       <c r="L34">
         <v>1.7158071456138699</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M34" s="1">
+        <v>4.7405399999999999E-7</v>
+      </c>
+      <c r="N34" s="1">
+        <f t="shared" ref="N34:N65" si="4">M34/I34</f>
+        <v>1.1493034448469353</v>
+      </c>
+      <c r="O34" s="1">
+        <f t="shared" ref="O34:O57" si="5">M34/J34</f>
+        <v>1.2110973827051166</v>
+      </c>
+      <c r="P34" s="1"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>2</v>
       </c>
@@ -10548,8 +12018,20 @@
       <c r="L35">
         <v>5.0953090287596901</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M35" s="1">
+        <v>1.0111999999999999E-7</v>
+      </c>
+      <c r="N35" s="1">
+        <f t="shared" si="4"/>
+        <v>2.2307123737713748</v>
+      </c>
+      <c r="O35" s="1">
+        <f t="shared" si="5"/>
+        <v>2.661488666484602</v>
+      </c>
+      <c r="P35" s="1"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>3</v>
       </c>
@@ -10586,8 +12068,20 @@
       <c r="L36">
         <v>1.6004128876108801</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M36" s="1">
+        <v>1.2976789999999999E-6</v>
+      </c>
+      <c r="N36" s="1">
+        <f t="shared" si="4"/>
+        <v>2.3137370544791911</v>
+      </c>
+      <c r="O36" s="1">
+        <f t="shared" si="5"/>
+        <v>2.2982517318090325</v>
+      </c>
+      <c r="P36" s="1"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -10624,8 +12118,20 @@
       <c r="L37">
         <v>2.9448290912564001</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M37" s="1">
+        <v>1.148579E-6</v>
+      </c>
+      <c r="N37" s="1">
+        <f t="shared" si="4"/>
+        <v>3.217224517373197</v>
+      </c>
+      <c r="O37" s="1">
+        <f t="shared" si="5"/>
+        <v>3.2150231770581983</v>
+      </c>
+      <c r="P37" s="1"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -10662,8 +12168,20 @@
       <c r="L38">
         <v>1.28091623410449</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M38" s="1">
+        <v>3.1489399999999999E-7</v>
+      </c>
+      <c r="N38" s="1">
+        <f t="shared" si="4"/>
+        <v>0.86735291380307455</v>
+      </c>
+      <c r="O38" s="1">
+        <f t="shared" si="5"/>
+        <v>0.97745607103916976</v>
+      </c>
+      <c r="P38" s="1"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -10700,8 +12218,20 @@
       <c r="L39">
         <v>4.3187854332005298</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M39" s="1">
+        <v>1.5592300000000001E-7</v>
+      </c>
+      <c r="N39" s="1">
+        <f t="shared" si="4"/>
+        <v>2.7403416863773646</v>
+      </c>
+      <c r="O39" s="1">
+        <f t="shared" si="5"/>
+        <v>3.3506583319124381</v>
+      </c>
+      <c r="P39" s="1"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -10738,8 +12268,20 @@
       <c r="L40">
         <v>1.5773826774292099</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M40" s="1">
+        <v>3.5330399E-5</v>
+      </c>
+      <c r="N40" s="1">
+        <f t="shared" si="4"/>
+        <v>2.1865305235299424</v>
+      </c>
+      <c r="O40" s="1">
+        <f t="shared" si="5"/>
+        <v>2.1819302184910914</v>
+      </c>
+      <c r="P40" s="1"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>8</v>
       </c>
@@ -10776,8 +12318,20 @@
       <c r="L41">
         <v>4.7086873366947204</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M41" s="1">
+        <v>3.45248E-7</v>
+      </c>
+      <c r="N41" s="1">
+        <f t="shared" si="4"/>
+        <v>6.6707272493558172</v>
+      </c>
+      <c r="O41" s="1">
+        <f t="shared" si="5"/>
+        <v>8.0793333076236493</v>
+      </c>
+      <c r="P41" s="1"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>0</v>
       </c>
@@ -10814,8 +12368,20 @@
       <c r="L42">
         <v>1.7251048461160401</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M42" s="1">
+        <v>5.0572400000000001E-7</v>
+      </c>
+      <c r="N42" s="1">
+        <f t="shared" si="4"/>
+        <v>1.3262259054619026</v>
+      </c>
+      <c r="O42" s="1">
+        <f t="shared" si="5"/>
+        <v>1.3119943148584194</v>
+      </c>
+      <c r="P42" s="1"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>2</v>
       </c>
@@ -10852,8 +12418,20 @@
       <c r="L43">
         <v>4.8100122357692099</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M43" s="1">
+        <v>1.27199E-7</v>
+      </c>
+      <c r="N43" s="1">
+        <f t="shared" si="4"/>
+        <v>3.4425554778256386</v>
+      </c>
+      <c r="O43" s="1">
+        <f t="shared" si="5"/>
+        <v>3.4544961145736641</v>
+      </c>
+      <c r="P43" s="1"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>3</v>
       </c>
@@ -10890,8 +12468,20 @@
       <c r="L44">
         <v>1.5541979421974701</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M44" s="1">
+        <v>1.299222E-6</v>
+      </c>
+      <c r="N44" s="1">
+        <f t="shared" si="4"/>
+        <v>2.1944412570088994</v>
+      </c>
+      <c r="O44" s="1">
+        <f t="shared" si="5"/>
+        <v>2.2531785005239588</v>
+      </c>
+      <c r="P44" s="1"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>4</v>
       </c>
@@ -10928,8 +12518,20 @@
       <c r="L45">
         <v>2.9291733683782999</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M45" s="1">
+        <v>1.091798E-6</v>
+      </c>
+      <c r="N45" s="1">
+        <f t="shared" si="4"/>
+        <v>3.0716361076565462</v>
+      </c>
+      <c r="O45" s="1">
+        <f t="shared" si="5"/>
+        <v>3.0690406353223292</v>
+      </c>
+      <c r="P45" s="1"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>5</v>
       </c>
@@ -10966,8 +12568,20 @@
       <c r="L46">
         <v>1.2214203288927701</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M46" s="1">
+        <v>3.2825500000000002E-7</v>
+      </c>
+      <c r="N46" s="1">
+        <f t="shared" si="4"/>
+        <v>0.84052651509527643</v>
+      </c>
+      <c r="O46" s="1">
+        <f t="shared" si="5"/>
+        <v>1.0186136677113617</v>
+      </c>
+      <c r="P46" s="1"/>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>6</v>
       </c>
@@ -11004,8 +12618,20 @@
       <c r="L47">
         <v>4.0958749952908402</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M47" s="1">
+        <v>1.5615300000000001E-7</v>
+      </c>
+      <c r="N47" s="1">
+        <f t="shared" si="4"/>
+        <v>3.475381462400795</v>
+      </c>
+      <c r="O47" s="1">
+        <f t="shared" si="5"/>
+        <v>3.4715734259661311</v>
+      </c>
+      <c r="P47" s="1"/>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>7</v>
       </c>
@@ -11042,8 +12668,20 @@
       <c r="L48">
         <v>2.2265545259281301</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M48" s="1">
+        <v>3.4860244999999998E-5</v>
+      </c>
+      <c r="N48" s="1">
+        <f t="shared" si="4"/>
+        <v>1.2475666379838264</v>
+      </c>
+      <c r="O48" s="1">
+        <f t="shared" si="5"/>
+        <v>2.2820323606948096</v>
+      </c>
+      <c r="P48" s="1"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>8</v>
       </c>
@@ -11080,8 +12718,20 @@
       <c r="L49">
         <v>4.47738548041852</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M49" s="1">
+        <v>3.2212500000000001E-7</v>
+      </c>
+      <c r="N49" s="1">
+        <f t="shared" si="4"/>
+        <v>7.2655506607929521</v>
+      </c>
+      <c r="O49" s="1">
+        <f t="shared" si="5"/>
+        <v>7.8419571847267822</v>
+      </c>
+      <c r="P49" s="1"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>0</v>
       </c>
@@ -11118,8 +12768,20 @@
       <c r="L50">
         <v>1.7109005628626399</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M50" s="1">
+        <v>4.8919799999999996E-7</v>
+      </c>
+      <c r="N50" s="1">
+        <f t="shared" si="4"/>
+        <v>1.2575359350193687</v>
+      </c>
+      <c r="O50" s="1">
+        <f t="shared" si="5"/>
+        <v>1.2786789248833876</v>
+      </c>
+      <c r="P50" s="1"/>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>2</v>
       </c>
@@ -11156,8 +12818,20 @@
       <c r="L51">
         <v>4.6066734252416301</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M51" s="1">
+        <v>1.11631E-7</v>
+      </c>
+      <c r="N51" s="1">
+        <f t="shared" si="4"/>
+        <v>3.0845330483159361</v>
+      </c>
+      <c r="O51" s="1">
+        <f t="shared" si="5"/>
+        <v>3.0508701022329516</v>
+      </c>
+      <c r="P51" s="1"/>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>3</v>
       </c>
@@ -11194,8 +12868,20 @@
       <c r="L52">
         <v>1.48612678803252</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M52" s="1">
+        <v>1.303459E-6</v>
+      </c>
+      <c r="N52" s="1">
+        <f t="shared" si="4"/>
+        <v>2.1993227748696826</v>
+      </c>
+      <c r="O52" s="1">
+        <f t="shared" si="5"/>
+        <v>2.2205758814548968</v>
+      </c>
+      <c r="P52" s="1"/>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>4</v>
       </c>
@@ -11232,8 +12918,20 @@
       <c r="L53">
         <v>2.8927501640876301</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M53" s="1">
+        <v>1.0949239999999999E-6</v>
+      </c>
+      <c r="N53" s="1">
+        <f t="shared" si="4"/>
+        <v>2.9847579622001907</v>
+      </c>
+      <c r="O53" s="1">
+        <f t="shared" si="5"/>
+        <v>3.1177251828743775</v>
+      </c>
+      <c r="P53" s="1"/>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>5</v>
       </c>
@@ -11270,8 +12968,20 @@
       <c r="L54">
         <v>1.21077611633966</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M54" s="1">
+        <v>3.2901699999999999E-7</v>
+      </c>
+      <c r="N54" s="1">
+        <f t="shared" si="4"/>
+        <v>0.84780251567331943</v>
+      </c>
+      <c r="O54" s="1">
+        <f t="shared" si="5"/>
+        <v>1.0345162358552891</v>
+      </c>
+      <c r="P54" s="1"/>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>6</v>
       </c>
@@ -11308,8 +13018,20 @@
       <c r="L55">
         <v>3.7555328665768202</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M55" s="1">
+        <v>1.5732699999999999E-7</v>
+      </c>
+      <c r="N55" s="1">
+        <f t="shared" si="4"/>
+        <v>3.6218656549902346</v>
+      </c>
+      <c r="O55" s="1">
+        <f t="shared" si="5"/>
+        <v>3.5102543248419091</v>
+      </c>
+      <c r="P55" s="1"/>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>7</v>
       </c>
@@ -11346,8 +13068,20 @@
       <c r="L56">
         <v>3.5378317641086401</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M56" s="1">
+        <v>3.0722546000000002E-5</v>
+      </c>
+      <c r="N56" s="1">
+        <f t="shared" si="4"/>
+        <v>1.9259080719716639</v>
+      </c>
+      <c r="O56" s="1">
+        <f t="shared" si="5"/>
+        <v>2.053171791489989</v>
+      </c>
+      <c r="P56" s="1"/>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>8</v>
       </c>
@@ -11384,8 +13118,20 @@
       <c r="L57">
         <v>4.2205166387267496</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M57" s="1">
+        <v>3.2071000000000002E-7</v>
+      </c>
+      <c r="N57" s="1">
+        <f t="shared" si="4"/>
+        <v>6.6492197229973051</v>
+      </c>
+      <c r="O57" s="1">
+        <f t="shared" si="5"/>
+        <v>7.7601910173549804</v>
+      </c>
+      <c r="P57" s="1"/>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
@@ -11423,7 +13169,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A91867BA-EC23-43F1-8D56-2CF4F5197532}">
   <dimension ref="A1:S57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -14171,23 +15917,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="fa0ea87a-dbc3-4034-822b-3be66bb1e531" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010099D54ACDED4E3145A16FA21A42E9B07A" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="53180cc22209dee855e9c7995086d4f8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fa0ea87a-dbc3-4034-822b-3be66bb1e531" xmlns:ns4="7581f031-74d9-476d-ad66-b7e2309b571d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="24aba60c41fd01c4f52a557d4e076795" ns3:_="" ns4:_="">
     <xsd:import namespace="fa0ea87a-dbc3-4034-822b-3be66bb1e531"/>
@@ -14420,32 +16149,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E400D861-C791-4665-80C3-5EFD5FFDF0DD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="7581f031-74d9-476d-ad66-b7e2309b571d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="fa0ea87a-dbc3-4034-822b-3be66bb1e531"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8E14463-0D0F-4755-9C80-F057C9F40301}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="fa0ea87a-dbc3-4034-822b-3be66bb1e531" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0B81907-87F3-49C0-BBBD-39556EDA75E2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14462,4 +16183,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8E14463-0D0F-4755-9C80-F057C9F40301}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E400D861-C791-4665-80C3-5EFD5FFDF0DD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="7581f031-74d9-476d-ad66-b7e2309b571d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="fa0ea87a-dbc3-4034-822b-3be66bb1e531"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>